<commit_message>
Adding test data from excel
</commit_message>
<xml_diff>
--- a/cypress/fixtures/StoresZipCodes.xlsx
+++ b/cypress/fixtures/StoresZipCodes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306498A4-9A72-419E-AD9D-22B8B7CA5638}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F314103-5A3C-48DE-92B4-44D938745B9A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>StoresList</t>
+    <t>Philadelphia, PA, USA</t>
   </si>
   <si>
-    <t>Philadelphia, PA, USA</t>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://dev01.ip.wawa.com/commerce/ui/</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
 </sst>
 </file>
@@ -84,10 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,25 +375,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>